<commit_message>
All tests and documents for loadrunner
</commit_message>
<xml_diff>
--- a/Документация/WebTours Профиль нагрузки WebTors.xlsx
+++ b/Документация/WebTours Профиль нагрузки WebTors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Load Testing XSET\Load-Testing-XSET\Документация\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C1C612-E5B3-4C8B-B6A1-A43467D3C0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F8F763-31A6-4192-9339-6D1E0E5A6979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4635" yWindow="6210" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Автоматизированный расчет" sheetId="3" r:id="rId1"/>
@@ -412,9 +412,6 @@
     <t>% Распределения пользователей</t>
   </si>
   <si>
-    <t>Всего пользователей на ступени</t>
-  </si>
-  <si>
     <t>Сумма по полю Итого</t>
   </si>
   <si>
@@ -572,6 +569,9 @@
   </si>
   <si>
     <t>UC_05_CancelingFlight</t>
+  </si>
+  <si>
+    <t>Количество выполнений в час</t>
   </si>
 </sst>
 </file>
@@ -1753,7 +1753,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1902,6 +1902,7 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="65"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1911,7 +1912,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="65"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="85">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2756,8 +2757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,13 +2794,13 @@
         <v>40</v>
       </c>
       <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>51</v>
-      </c>
-      <c r="G1" t="s">
-        <v>52</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -2808,7 +2809,7 @@
         <v>37</v>
       </c>
       <c r="J1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M1" t="s">
         <v>39</v>
@@ -2820,7 +2821,7 @@
         <v>42</v>
       </c>
       <c r="P1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q1" t="s">
         <v>43</v>
@@ -2841,15 +2842,15 @@
         <v>47</v>
       </c>
       <c r="X1" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="88" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="85" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="67">
         <v>1</v>
@@ -2881,7 +2882,7 @@
       </c>
       <c r="K2" s="15"/>
       <c r="M2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N2" s="23">
         <v>1.7749999999999999</v>
@@ -2918,10 +2919,14 @@
         <f>SUM(R2:R7)</f>
         <v>10</v>
       </c>
+      <c r="X2" s="102">
+        <f xml:space="preserve"> 3600 / Q2</f>
+        <v>58.064516129032256</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="86" t="s">
         <v>0</v>
@@ -2956,7 +2961,7 @@
       </c>
       <c r="K3" s="15"/>
       <c r="M3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N3" s="23">
         <v>1.62</v>
@@ -2989,10 +2994,14 @@
         <f>R3/W$2</f>
         <v>0.1</v>
       </c>
+      <c r="X3" s="102">
+        <f t="shared" ref="X3:X7" si="7" xml:space="preserve"> 3600 / Q3</f>
+        <v>72</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="86" t="s">
         <v>4</v>
@@ -3027,7 +3036,7 @@
       </c>
       <c r="K4" s="15"/>
       <c r="M4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N4" s="23">
         <v>2.9750000000000001</v>
@@ -3057,13 +3066,17 @@
         <v>32</v>
       </c>
       <c r="V4" s="38">
-        <f t="shared" ref="V4:V5" si="7">R4/W$2</f>
+        <f t="shared" ref="V4:V5" si="8">R4/W$2</f>
         <v>0.1</v>
+      </c>
+      <c r="X4" s="102">
+        <f t="shared" si="7"/>
+        <v>97.297297297297291</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="95" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="93" t="s">
         <v>6</v>
@@ -3098,7 +3111,7 @@
       </c>
       <c r="K5" s="15"/>
       <c r="M5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N5" s="23">
         <v>1.2390000000000001</v>
@@ -3128,22 +3141,26 @@
         <v>34</v>
       </c>
       <c r="V5" s="38">
+        <f t="shared" si="8"/>
+        <v>0.2</v>
+      </c>
+      <c r="X5" s="102">
         <f t="shared" si="7"/>
-        <v>0.2</v>
+        <v>50.70422535211268</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="85" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="66">
         <v>1</v>
       </c>
       <c r="D6" s="53">
-        <f t="shared" ref="D6:D34" si="8">VLOOKUP(A6,$M$1:$W$8,6,FALSE)</f>
+        <f t="shared" ref="D6:D34" si="9">VLOOKUP(A6,$M$1:$W$8,6,FALSE)</f>
         <v>1</v>
       </c>
       <c r="E6" s="70">
@@ -3151,7 +3168,7 @@
         <v>190</v>
       </c>
       <c r="F6" s="76">
-        <f t="shared" ref="F6:F34" si="9">60/E6*C6</f>
+        <f t="shared" ref="F6:F34" si="10">60/E6*C6</f>
         <v>0.31578947368421051</v>
       </c>
       <c r="G6" s="73">
@@ -3169,7 +3186,7 @@
       </c>
       <c r="K6" s="15"/>
       <c r="M6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N6" s="23">
         <v>1.107</v>
@@ -3202,10 +3219,14 @@
         <f>R6/W$2</f>
         <v>0.1</v>
       </c>
+      <c r="X6" s="102">
+        <f t="shared" si="7"/>
+        <v>18.94736842105263</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="89" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="86" t="s">
         <v>0</v>
@@ -3214,7 +3235,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E7" s="71">
@@ -3222,7 +3243,7 @@
         <v>190</v>
       </c>
       <c r="F7" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.31578947368421051</v>
       </c>
       <c r="G7" s="61">
@@ -3240,7 +3261,7 @@
       </c>
       <c r="K7" s="15"/>
       <c r="M7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N7" s="23">
         <v>0.70899999999999996</v>
@@ -3273,34 +3294,38 @@
         <f>R7/W$2</f>
         <v>0.2</v>
       </c>
+      <c r="X7" s="102">
+        <f t="shared" si="7"/>
+        <v>21.176470588235293</v>
+      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="89" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="86" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="29">
         <v>1</v>
       </c>
       <c r="D8" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E8" s="71">
-        <f t="shared" ref="E8:E9" si="10">VLOOKUP(A8,$M$1:$W$8,5,FALSE)</f>
+        <f t="shared" ref="E8:E9" si="11">VLOOKUP(A8,$M$1:$W$8,5,FALSE)</f>
         <v>190</v>
       </c>
       <c r="F8" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.31578947368421051</v>
       </c>
       <c r="G8" s="61">
         <v>20</v>
       </c>
       <c r="H8" s="78">
-        <f t="shared" ref="H8:H9" si="11">D8*F8*G8</f>
+        <f t="shared" ref="H8:H9" si="12">D8*F8*G8</f>
         <v>6.3157894736842106</v>
       </c>
       <c r="I8" s="17" t="s">
@@ -3315,13 +3340,17 @@
         <v>154</v>
       </c>
       <c r="V8" s="38">
-        <f>SUM(V2:V6)</f>
-        <v>0.79999999999999993</v>
+        <f>SUM(V2:V7)</f>
+        <v>1</v>
+      </c>
+      <c r="X8" s="102">
+        <f>SUM(X2:X7)</f>
+        <v>318.18987778773015</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="89" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="86" t="s">
         <v>8</v>
@@ -3330,26 +3359,26 @@
         <v>1</v>
       </c>
       <c r="D9" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E9" s="71">
+        <f t="shared" si="11"/>
+        <v>190</v>
+      </c>
+      <c r="F9" s="75">
         <f t="shared" si="10"/>
-        <v>190</v>
-      </c>
-      <c r="F9" s="75">
-        <f t="shared" si="9"/>
         <v>0.31578947368421051</v>
       </c>
       <c r="G9" s="61">
         <v>20</v>
       </c>
       <c r="H9" s="78">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6.3157894736842106</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" s="15">
         <v>168.73320199538091</v>
@@ -3358,7 +3387,7 @@
     </row>
     <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="90" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="87" t="s">
         <v>6</v>
@@ -3367,26 +3396,26 @@
         <v>0</v>
       </c>
       <c r="D10" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E10" s="72">
-        <f t="shared" ref="E10:E34" si="12">VLOOKUP(A10,$M$1:$W$8,5,FALSE)</f>
+        <f t="shared" ref="E10:E34" si="13">VLOOKUP(A10,$M$1:$W$8,5,FALSE)</f>
         <v>190</v>
       </c>
       <c r="F10" s="79">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G10" s="74">
         <v>20</v>
       </c>
       <c r="H10" s="80">
-        <f t="shared" ref="H10:H34" si="13">D10*F10*G10</f>
+        <f t="shared" ref="H10:H34" si="14">D10*F10*G10</f>
         <v>0</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J10" s="15">
         <v>32.432432432432435</v>
@@ -3394,35 +3423,35 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="88" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="85" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="67">
         <v>1</v>
       </c>
       <c r="D11" s="62">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="E11" s="73">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>71</v>
       </c>
       <c r="F11" s="76">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.84507042253521125</v>
       </c>
       <c r="G11" s="73">
         <v>20</v>
       </c>
       <c r="H11" s="77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>33.802816901408448</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J11" s="15">
         <v>32.432432432432435</v>
@@ -3430,7 +3459,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" s="86" t="s">
         <v>0</v>
@@ -3439,26 +3468,26 @@
         <v>1</v>
       </c>
       <c r="D12" s="63">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="E12" s="61">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>71</v>
       </c>
       <c r="F12" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.84507042253521125</v>
       </c>
       <c r="G12" s="61">
         <v>20</v>
       </c>
       <c r="H12" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>33.802816901408448</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J12" s="15">
         <v>32.432432432432435</v>
@@ -3466,35 +3495,35 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" s="86" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="60">
         <v>1</v>
       </c>
       <c r="D13" s="63">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="E13" s="61">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>71</v>
       </c>
       <c r="F13" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.84507042253521125</v>
       </c>
       <c r="G13" s="61">
         <v>20</v>
       </c>
       <c r="H13" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>33.802816901408448</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13" s="15">
         <v>98.183122504124924</v>
@@ -3502,7 +3531,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" s="86" t="s">
         <v>8</v>
@@ -3511,22 +3540,22 @@
         <v>1</v>
       </c>
       <c r="D14" s="63">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="E14" s="61">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>71</v>
       </c>
       <c r="F14" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.84507042253521125</v>
       </c>
       <c r="G14" s="61">
         <v>20</v>
       </c>
       <c r="H14" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>33.802816901408448</v>
       </c>
       <c r="I14" s="17" t="s">
@@ -3538,7 +3567,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" s="86" t="s">
         <v>9</v>
@@ -3547,28 +3576,28 @@
         <v>1</v>
       </c>
       <c r="D15" s="63">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="E15" s="61">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>71</v>
       </c>
       <c r="F15" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.84507042253521125</v>
       </c>
       <c r="G15" s="61">
         <v>20</v>
       </c>
       <c r="H15" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>33.802816901408448</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="95" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="87" t="s">
         <v>6</v>
@@ -3577,88 +3606,88 @@
         <v>1</v>
       </c>
       <c r="D16" s="64">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="E16" s="74">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>71</v>
       </c>
       <c r="F16" s="79">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.84507042253521125</v>
       </c>
       <c r="G16" s="74">
         <v>20</v>
       </c>
       <c r="H16" s="80">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>33.802816901408448</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="85" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="66">
         <v>1</v>
       </c>
       <c r="D17" s="53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="E17" s="70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>62</v>
       </c>
       <c r="F17" s="76">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.967741935483871</v>
       </c>
       <c r="G17" s="73">
         <v>20</v>
       </c>
       <c r="H17" s="77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>58.064516129032256</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="89" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B18" s="86" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="29">
         <v>1</v>
       </c>
       <c r="D18" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="E18" s="71">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>62</v>
       </c>
       <c r="F18" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.967741935483871</v>
       </c>
       <c r="G18" s="61">
         <v>20</v>
       </c>
       <c r="H18" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>58.064516129032256</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="89" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="86" t="s">
         <v>0</v>
@@ -3667,28 +3696,28 @@
         <v>1</v>
       </c>
       <c r="D19" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="E19" s="71">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>62</v>
       </c>
       <c r="F19" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.967741935483871</v>
       </c>
       <c r="G19" s="61">
         <v>20</v>
       </c>
       <c r="H19" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>58.064516129032256</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="89" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" s="86" t="s">
         <v>8</v>
@@ -3697,28 +3726,28 @@
         <v>1</v>
       </c>
       <c r="D20" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="E20" s="71">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>62</v>
       </c>
       <c r="F20" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.967741935483871</v>
       </c>
       <c r="G20" s="61">
         <v>20</v>
       </c>
       <c r="H20" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>58.064516129032256</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="89" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="86" t="s">
         <v>9</v>
@@ -3727,28 +3756,28 @@
         <v>1</v>
       </c>
       <c r="D21" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="E21" s="71">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>62</v>
       </c>
       <c r="F21" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.967741935483871</v>
       </c>
       <c r="G21" s="61">
         <v>20</v>
       </c>
       <c r="H21" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>58.064516129032256</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="89" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" s="86" t="s">
         <v>3</v>
@@ -3757,28 +3786,28 @@
         <v>1</v>
       </c>
       <c r="D22" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="E22" s="71">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>62</v>
       </c>
       <c r="F22" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.967741935483871</v>
       </c>
       <c r="G22" s="61">
         <v>20</v>
       </c>
       <c r="H22" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>58.064516129032256</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="89" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="86" t="s">
         <v>4</v>
@@ -3787,28 +3816,28 @@
         <v>1</v>
       </c>
       <c r="D23" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="E23" s="71">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>62</v>
       </c>
       <c r="F23" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.967741935483871</v>
       </c>
       <c r="G23" s="61">
         <v>20</v>
       </c>
       <c r="H23" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>58.064516129032256</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="90" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="87" t="s">
         <v>6</v>
@@ -3817,58 +3846,58 @@
         <v>1</v>
       </c>
       <c r="D24" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="E24" s="72">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>62</v>
       </c>
       <c r="F24" s="79">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.967741935483871</v>
       </c>
       <c r="G24" s="74">
         <v>20</v>
       </c>
       <c r="H24" s="80">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>58.064516129032256</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="88" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="94" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="65">
         <v>1</v>
       </c>
       <c r="D25" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E25" s="82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="F25" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2</v>
       </c>
       <c r="G25" s="61">
         <v>20</v>
       </c>
       <c r="H25" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="86" t="s">
         <v>0</v>
@@ -3877,28 +3906,28 @@
         <v>1</v>
       </c>
       <c r="D26" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E26" s="82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="F26" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2</v>
       </c>
       <c r="G26" s="61">
         <v>20</v>
       </c>
       <c r="H26" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" s="86" t="s">
         <v>4</v>
@@ -3907,28 +3936,28 @@
         <v>1</v>
       </c>
       <c r="D27" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E27" s="82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="F27" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2</v>
       </c>
       <c r="G27" s="61">
         <v>20</v>
       </c>
       <c r="H27" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B28" s="86" t="s">
         <v>10</v>
@@ -3937,28 +3966,28 @@
         <v>1</v>
       </c>
       <c r="D28" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E28" s="82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="F28" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2</v>
       </c>
       <c r="G28" s="61">
         <v>20</v>
       </c>
       <c r="H28" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="97" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29" s="87" t="s">
         <v>6</v>
@@ -3967,148 +3996,148 @@
         <v>0</v>
       </c>
       <c r="D29" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E29" s="83">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="F29" s="79">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G29" s="74">
         <v>20</v>
       </c>
       <c r="H29" s="80">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="96" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B30" s="94" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="65">
         <v>1</v>
       </c>
       <c r="D30" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E30" s="81">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>37</v>
       </c>
       <c r="F30" s="76">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.6216216216216217</v>
       </c>
       <c r="G30" s="73">
         <v>20</v>
       </c>
       <c r="H30" s="77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>32.432432432432435</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="96" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B31" s="86" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="29">
         <v>1</v>
       </c>
       <c r="D31" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E31" s="82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>37</v>
       </c>
       <c r="F31" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.6216216216216217</v>
       </c>
       <c r="G31" s="61">
         <v>20</v>
       </c>
       <c r="H31" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>32.432432432432435</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="96" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B32" s="86" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="29">
         <v>1</v>
       </c>
       <c r="D32" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E32" s="82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>37</v>
       </c>
       <c r="F32" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.6216216216216217</v>
       </c>
       <c r="G32" s="61">
         <v>20</v>
       </c>
       <c r="H32" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>32.432432432432435</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="96" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B33" s="86" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" s="29">
         <v>1</v>
       </c>
       <c r="D33" s="51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E33" s="82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>37</v>
       </c>
       <c r="F33" s="75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.6216216216216217</v>
       </c>
       <c r="G33" s="61">
         <v>20</v>
       </c>
       <c r="H33" s="78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>32.432432432432435</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="97" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" s="86" t="s">
         <v>6</v>
@@ -4117,71 +4146,71 @@
         <v>0</v>
       </c>
       <c r="D34" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E34" s="83">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>37</v>
       </c>
       <c r="F34" s="79">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G34" s="74">
         <v>20</v>
       </c>
       <c r="H34" s="80">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="98" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" s="99"/>
+      <c r="A44" s="99" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="100"/>
     </row>
     <row r="45" spans="1:8" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A45" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B45" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="E45" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G45" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="D45" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="E45" s="58" t="s">
-        <v>81</v>
-      </c>
-      <c r="F45" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="G45" s="28" t="s">
+      <c r="H45" s="28" t="s">
         <v>58</v>
-      </c>
-      <c r="H45" s="28" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46" s="43">
         <v>520</v>
       </c>
       <c r="C46" s="27">
-        <f t="shared" ref="C46:C57" si="14">GETPIVOTDATA("Итого",$I$1,"transaction rq",A46)*3</f>
+        <f t="shared" ref="C46:C57" si="15">GETPIVOTDATA("Итого",$I$1,"transaction rq",A46)*3</f>
         <v>506.19960598614273</v>
       </c>
       <c r="D46" s="57">
-        <f t="shared" ref="D46:D58" si="15">1-B46/C46</f>
+        <f t="shared" ref="D46:D58" si="16">1-B46/C46</f>
         <v>-2.7262751394229845E-2</v>
       </c>
       <c r="E46" s="55" t="str">
@@ -4189,7 +4218,7 @@
         <v>openHomePage</v>
       </c>
       <c r="F46" s="59">
-        <f t="shared" ref="F46:F57" si="16">C46/3</f>
+        <f t="shared" ref="F46:F57" si="17">C46/3</f>
         <v>168.73320199538091</v>
       </c>
       <c r="G46" s="50">
@@ -4209,11 +4238,11 @@
         <v>422</v>
       </c>
       <c r="C47" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>408.90230868884538</v>
       </c>
       <c r="D47" s="57">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.2031345954373958E-2</v>
       </c>
       <c r="E47" s="55" t="str">
@@ -4221,7 +4250,7 @@
         <v>login</v>
       </c>
       <c r="F47" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>136.30076956294846</v>
       </c>
       <c r="G47" s="50">
@@ -4235,17 +4264,17 @@
     </row>
     <row r="48" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" s="43">
         <v>305</v>
       </c>
       <c r="C48" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>294.54936751237477</v>
       </c>
       <c r="D48" s="57">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-3.5480071051879447E-2</v>
       </c>
       <c r="E48" s="55" t="str">
@@ -4253,7 +4282,7 @@
         <v>flightsBottonClick</v>
       </c>
       <c r="F48" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>98.183122504124924</v>
       </c>
       <c r="G48" s="50">
@@ -4273,11 +4302,11 @@
         <v>282</v>
       </c>
       <c r="C49" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>294.54936751237477</v>
       </c>
       <c r="D49" s="54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.2605311355311426E-2</v>
       </c>
       <c r="E49" s="55" t="str">
@@ -4285,7 +4314,7 @@
         <v>startFindingFlights</v>
       </c>
       <c r="F49" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>98.183122504124924</v>
       </c>
       <c r="G49" s="50">
@@ -4293,7 +4322,7 @@
         <v>98</v>
       </c>
       <c r="H49" s="25">
-        <f t="shared" ref="H49:H57" si="17">1-F49/G49</f>
+        <f t="shared" ref="H49:H57" si="18">1-F49/G49</f>
         <v>-1.8685969808664993E-3</v>
       </c>
     </row>
@@ -4305,11 +4334,11 @@
         <v>270</v>
       </c>
       <c r="C50" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>275.60199909132211</v>
       </c>
       <c r="D50" s="54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.0326409495548869E-2</v>
       </c>
       <c r="E50" s="55" t="str">
@@ -4317,7 +4346,7 @@
         <v>choseFlightTime</v>
       </c>
       <c r="F50" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>91.867333030440705</v>
       </c>
       <c r="G50" s="50">
@@ -4325,7 +4354,7 @@
         <v>92</v>
       </c>
       <c r="H50" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.4420322778184724E-3</v>
       </c>
     </row>
@@ -4337,11 +4366,11 @@
         <v>175</v>
       </c>
       <c r="C51" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>174.19354838709677</v>
       </c>
       <c r="D51" s="54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-4.6296296296297612E-3</v>
       </c>
       <c r="E51" s="55" t="str">
@@ -4349,7 +4378,7 @@
         <v>paymentDetails</v>
       </c>
       <c r="F51" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>58.064516129032256</v>
       </c>
       <c r="G51" s="50">
@@ -4357,7 +4386,7 @@
         <v>58</v>
       </c>
       <c r="H51" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-1.1123470522802492E-3</v>
       </c>
     </row>
@@ -4369,11 +4398,11 @@
         <v>280</v>
       </c>
       <c r="C52" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>288.54648956356738</v>
       </c>
       <c r="D52" s="54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.9619107744107809E-2</v>
       </c>
       <c r="E52" s="55" t="str">
@@ -4381,7 +4410,7 @@
         <v>browsingItenerary</v>
       </c>
       <c r="F52" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>96.182163187855792</v>
       </c>
       <c r="G52" s="50">
@@ -4389,7 +4418,7 @@
         <v>97</v>
       </c>
       <c r="H52" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8.4313073416928397E-3</v>
       </c>
     </row>
@@ -4401,11 +4430,11 @@
         <v>73</v>
       </c>
       <c r="C53" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>72</v>
       </c>
       <c r="D53" s="54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-1.388888888888884E-2</v>
       </c>
       <c r="E53" s="55" t="str">
@@ -4413,7 +4442,7 @@
         <v>CancelingFlight</v>
       </c>
       <c r="F53" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>24</v>
       </c>
       <c r="G53" s="50">
@@ -4421,7 +4450,7 @@
         <v>24</v>
       </c>
       <c r="H53" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -4433,11 +4462,11 @@
         <v>326</v>
       </c>
       <c r="C54" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>317.95494026779272</v>
       </c>
       <c r="D54" s="54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-2.5302515272860537E-2</v>
       </c>
       <c r="E54" s="55" t="str">
@@ -4445,7 +4474,7 @@
         <v>logout</v>
       </c>
       <c r="F54" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>105.98498008926424</v>
       </c>
       <c r="G54" s="50">
@@ -4453,23 +4482,23 @@
         <v>107</v>
       </c>
       <c r="H54" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.4861673900538124E-3</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A55" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B55" s="43">
         <v>97</v>
       </c>
       <c r="C55" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97.297297297297305</v>
       </c>
       <c r="D55" s="54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.0555555555555891E-3</v>
       </c>
       <c r="E55" s="55" t="str">
@@ -4477,7 +4506,7 @@
         <v>signUpNowButtonClick</v>
       </c>
       <c r="F55" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>32.432432432432435</v>
       </c>
       <c r="G55" s="50">
@@ -4485,23 +4514,23 @@
         <v>32</v>
       </c>
       <c r="H55" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-1.3513513513513598E-2</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A56" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56" s="43">
         <v>97</v>
       </c>
       <c r="C56" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97.297297297297305</v>
       </c>
       <c r="D56" s="54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.0555555555555891E-3</v>
       </c>
       <c r="E56" s="55" t="str">
@@ -4509,7 +4538,7 @@
         <v>newUserRegistration</v>
       </c>
       <c r="F56" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>32.432432432432435</v>
       </c>
       <c r="G56" s="50">
@@ -4517,23 +4546,23 @@
         <v>32</v>
       </c>
       <c r="H56" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-1.3513513513513598E-2</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" s="43">
         <v>97</v>
       </c>
       <c r="C57" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>97.297297297297305</v>
       </c>
       <c r="D57" s="54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.0555555555555891E-3</v>
       </c>
       <c r="E57" s="55" t="str">
@@ -4541,7 +4570,7 @@
         <v>continueButtonClick</v>
       </c>
       <c r="F57" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>32.432432432432435</v>
       </c>
       <c r="G57" s="50">
@@ -4549,7 +4578,7 @@
         <v>32</v>
       </c>
       <c r="H57" s="25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-1.3513513513513598E-2</v>
       </c>
     </row>
@@ -4566,13 +4595,13 @@
         <v>2924.3895189014092</v>
       </c>
       <c r="D58" s="24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-6.7058375677524484E-3</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C69" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D69" s="34"/>
       <c r="E69" s="34"/>
@@ -4582,30 +4611,30 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D70" t="s">
+        <v>68</v>
+      </c>
+      <c r="E70" t="s">
+        <v>70</v>
+      </c>
+      <c r="F70" t="s">
         <v>69</v>
       </c>
-      <c r="E70" t="s">
+      <c r="G70" t="s">
         <v>71</v>
       </c>
-      <c r="F70" t="s">
-        <v>70</v>
-      </c>
-      <c r="G70" t="s">
-        <v>72</v>
-      </c>
       <c r="H70" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B71" s="35">
         <f>124/3</f>
@@ -4640,7 +4669,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B72" s="35">
         <f>150/3</f>
@@ -4650,7 +4679,7 @@
         <v>25</v>
       </c>
       <c r="D72" s="35">
-        <f t="shared" ref="D72:D75" si="18">60/C72</f>
+        <f t="shared" ref="D72:D75" si="19">60/C72</f>
         <v>2.4</v>
       </c>
       <c r="E72" s="49">
@@ -4661,11 +4690,11 @@
         <v>1.0416666666666667</v>
       </c>
       <c r="G72" s="20">
-        <f t="shared" ref="G72:G75" si="19">ROUND(F72,0)</f>
+        <f t="shared" ref="G72:G75" si="20">ROUND(F72,0)</f>
         <v>1</v>
       </c>
       <c r="H72" s="20">
-        <f t="shared" ref="H72:H75" si="20">G72*D72*E72</f>
+        <f t="shared" ref="H72:H75" si="21">G72*D72*E72</f>
         <v>48</v>
       </c>
       <c r="I72" s="33">
@@ -4675,7 +4704,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B73" s="36">
         <f>30/3</f>
@@ -4685,7 +4714,7 @@
         <v>115</v>
       </c>
       <c r="D73" s="35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.52173913043478259</v>
       </c>
       <c r="E73" s="49">
@@ -4699,7 +4728,7 @@
         <v>1</v>
       </c>
       <c r="H73" s="20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>10.434782608695652</v>
       </c>
       <c r="I73" s="33">
@@ -4709,7 +4738,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B74" s="35">
         <f>20/3</f>
@@ -4719,7 +4748,7 @@
         <v>180</v>
       </c>
       <c r="D74" s="35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E74" s="49">
@@ -4733,7 +4762,7 @@
         <v>1</v>
       </c>
       <c r="H74" s="20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6.6666666666666661</v>
       </c>
       <c r="I74" s="33">
@@ -4743,7 +4772,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B75" s="35">
         <f>120/3</f>
@@ -4753,7 +4782,7 @@
         <v>30</v>
       </c>
       <c r="D75" s="35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2</v>
       </c>
       <c r="E75" s="49">
@@ -4764,11 +4793,11 @@
         <v>1</v>
       </c>
       <c r="G75" s="20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="H75" s="20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>40</v>
       </c>
       <c r="I75" s="33">
@@ -4808,10 +4837,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4820,7 +4849,7 @@
         <v>Главная Welcome страница</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4838,7 +4867,7 @@
         <v>Переход на страницу поиска билетов</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4847,7 +4876,7 @@
         <v xml:space="preserve">Заполнение полей для поиска билета </v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4856,7 +4885,7 @@
         <v xml:space="preserve">Выбор рейса из найденных </v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4865,7 +4894,7 @@
         <v>Оплата билета</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4874,7 +4903,7 @@
         <v>Просмотр квитанций</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4883,7 +4912,7 @@
         <v xml:space="preserve">Отмена бронирования </v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4901,7 +4930,7 @@
         <v>Перход на страницу регистрации</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4910,7 +4939,7 @@
         <v>Заполнение полей регистарции</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4919,7 +4948,7 @@
         <v>Переход на следуюущий эран после регистарции</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -4942,578 +4971,578 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="98">
+        <v>0</v>
+      </c>
+      <c r="D1" s="98">
+        <v>0</v>
+      </c>
+      <c r="E1" s="98">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="F1" s="98">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="G1" s="98">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="H1" s="98">
+        <v>169</v>
+      </c>
+      <c r="I1" s="98">
+        <v>0</v>
+      </c>
+      <c r="J1" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="98" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="98">
+        <v>0</v>
+      </c>
+      <c r="D2" s="98">
+        <v>0</v>
+      </c>
+      <c r="E2" s="98">
+        <v>0.156</v>
+      </c>
+      <c r="F2" s="98">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G2" s="98">
+        <v>0.128</v>
+      </c>
+      <c r="H2" s="98">
+        <v>97</v>
+      </c>
+      <c r="I2" s="98">
+        <v>0</v>
+      </c>
+      <c r="J2" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="98" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="98">
+        <v>0</v>
+      </c>
+      <c r="D3" s="98">
+        <v>0</v>
+      </c>
+      <c r="E3" s="98">
+        <v>6.3E-2</v>
+      </c>
+      <c r="F3" s="98">
+        <v>0.01</v>
+      </c>
+      <c r="G3" s="98">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="H3" s="98">
+        <v>24</v>
+      </c>
+      <c r="I3" s="98">
+        <v>0</v>
+      </c>
+      <c r="J3" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="98">
+        <v>0</v>
+      </c>
+      <c r="D4" s="98">
+        <v>0</v>
+      </c>
+      <c r="E4" s="98">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F4" s="98">
+        <v>0.01</v>
+      </c>
+      <c r="G4" s="98">
+        <v>6.3E-2</v>
+      </c>
+      <c r="H4" s="98">
+        <v>92</v>
+      </c>
+      <c r="I4" s="98">
+        <v>0</v>
+      </c>
+      <c r="J4" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="98" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="98">
+        <v>0</v>
+      </c>
+      <c r="D5" s="98">
+        <v>0</v>
+      </c>
+      <c r="E5" s="98">
+        <v>0.123</v>
+      </c>
+      <c r="F5" s="98">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G5" s="98">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="H5" s="98">
+        <v>32</v>
+      </c>
+      <c r="I5" s="98">
+        <v>0</v>
+      </c>
+      <c r="J5" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="98" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="98">
+        <v>0</v>
+      </c>
+      <c r="D6" s="98">
+        <v>0</v>
+      </c>
+      <c r="E6" s="98">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="F6" s="98">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G6" s="98">
+        <v>0.128</v>
+      </c>
+      <c r="H6" s="98">
+        <v>98</v>
+      </c>
+      <c r="I6" s="98">
+        <v>0</v>
+      </c>
+      <c r="J6" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="98" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="98">
+        <v>0</v>
+      </c>
+      <c r="D7" s="98">
+        <v>0</v>
+      </c>
+      <c r="E7" s="98">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="F7" s="98">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G7" s="98">
+        <v>0.107</v>
+      </c>
+      <c r="H7" s="98">
+        <v>136</v>
+      </c>
+      <c r="I7" s="98">
+        <v>0</v>
+      </c>
+      <c r="J7" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="98" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="98">
+        <v>0</v>
+      </c>
+      <c r="D8" s="98">
+        <v>0</v>
+      </c>
+      <c r="E8" s="98">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="F8" s="98">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G8" s="98">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="98">
+        <v>107</v>
+      </c>
+      <c r="I8" s="98">
+        <v>0</v>
+      </c>
+      <c r="J8" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="98" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="98">
+        <v>0</v>
+      </c>
+      <c r="D9" s="98">
+        <v>0</v>
+      </c>
+      <c r="E9" s="98">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F9" s="98">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G9" s="98">
+        <v>6.3E-2</v>
+      </c>
+      <c r="H9" s="98">
+        <v>32</v>
+      </c>
+      <c r="I9" s="98">
+        <v>0</v>
+      </c>
+      <c r="J9" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="98" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="98">
+        <v>0</v>
+      </c>
+      <c r="D10" s="98">
+        <v>0</v>
+      </c>
+      <c r="E10" s="98">
+        <v>0.105</v>
+      </c>
+      <c r="F10" s="98">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G10" s="98">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="H10" s="98">
+        <v>169</v>
+      </c>
+      <c r="I10" s="98">
+        <v>0</v>
+      </c>
+      <c r="J10" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="98">
+        <v>0</v>
+      </c>
+      <c r="D11" s="98">
+        <v>0</v>
+      </c>
+      <c r="E11" s="98">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="F11" s="98">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G11" s="98">
+        <v>6.2E-2</v>
+      </c>
+      <c r="H11" s="98">
+        <v>58</v>
+      </c>
+      <c r="I11" s="98">
+        <v>0</v>
+      </c>
+      <c r="J11" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="98" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="98">
+        <v>0</v>
+      </c>
+      <c r="D12" s="98">
+        <v>0</v>
+      </c>
+      <c r="E12" s="98">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F12" s="98">
+        <v>0.01</v>
+      </c>
+      <c r="G12" s="98">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="H12" s="98">
+        <v>32</v>
+      </c>
+      <c r="I12" s="98">
+        <v>0</v>
+      </c>
+      <c r="J12" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="98" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="98">
+        <v>0</v>
+      </c>
+      <c r="D13" s="98">
+        <v>0</v>
+      </c>
+      <c r="E13" s="98">
+        <v>0.154</v>
+      </c>
+      <c r="F13" s="98">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G13" s="98">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="H13" s="98">
+        <v>98</v>
+      </c>
+      <c r="I13" s="98">
+        <v>0</v>
+      </c>
+      <c r="J13" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="98" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="101">
-        <v>0</v>
-      </c>
-      <c r="D1" s="101">
-        <v>0</v>
-      </c>
-      <c r="E1" s="101">
+      <c r="B14" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="98">
+        <v>0</v>
+      </c>
+      <c r="D14" s="98">
+        <v>0</v>
+      </c>
+      <c r="E14" s="98">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F14" s="98">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G14" s="98">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="H14" s="98">
+        <v>14</v>
+      </c>
+      <c r="I14" s="98">
+        <v>0</v>
+      </c>
+      <c r="J14" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="98" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="98">
+        <v>0</v>
+      </c>
+      <c r="D15" s="98">
+        <v>0</v>
+      </c>
+      <c r="E15" s="98">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="F15" s="98">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="G15" s="98">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="H15" s="98">
+        <v>6</v>
+      </c>
+      <c r="I15" s="98">
+        <v>0</v>
+      </c>
+      <c r="J15" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="98" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="98">
+        <v>0</v>
+      </c>
+      <c r="D16" s="98">
+        <v>0</v>
+      </c>
+      <c r="E16" s="98">
         <v>0.72799999999999998</v>
       </c>
-      <c r="F1" s="101">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="G1" s="101">
-        <v>0.63300000000000001</v>
-      </c>
-      <c r="H1" s="101">
-        <v>169</v>
-      </c>
-      <c r="I1" s="101">
-        <v>0</v>
-      </c>
-      <c r="J1" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="101" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="101">
-        <v>0</v>
-      </c>
-      <c r="D2" s="101">
-        <v>0</v>
-      </c>
-      <c r="E2" s="101">
-        <v>0.156</v>
-      </c>
-      <c r="F2" s="101">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="G2" s="101">
-        <v>0.128</v>
-      </c>
-      <c r="H2" s="101">
+      <c r="F16" s="98">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G16" s="98">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="H16" s="98">
+        <v>59</v>
+      </c>
+      <c r="I16" s="98">
+        <v>0</v>
+      </c>
+      <c r="J16" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="101">
-        <v>0</v>
-      </c>
-      <c r="J2" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="101" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="101">
-        <v>0</v>
-      </c>
-      <c r="D3" s="101">
-        <v>0</v>
-      </c>
-      <c r="E3" s="101">
-        <v>6.3E-2</v>
-      </c>
-      <c r="F3" s="101">
-        <v>0.01</v>
-      </c>
-      <c r="G3" s="101">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="H3" s="101">
+      <c r="B17" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="98">
+        <v>0</v>
+      </c>
+      <c r="D17" s="98">
+        <v>0</v>
+      </c>
+      <c r="E17" s="98">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="F17" s="98">
+        <v>3.1E-2</v>
+      </c>
+      <c r="G17" s="98">
+        <v>0.36</v>
+      </c>
+      <c r="H17" s="98">
         <v>24</v>
       </c>
-      <c r="I3" s="101">
-        <v>0</v>
-      </c>
-      <c r="J3" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="101" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="101">
-        <v>0</v>
-      </c>
-      <c r="D4" s="101">
-        <v>0</v>
-      </c>
-      <c r="E4" s="101">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="F4" s="101">
-        <v>0.01</v>
-      </c>
-      <c r="G4" s="101">
-        <v>6.3E-2</v>
-      </c>
-      <c r="H4" s="101">
-        <v>92</v>
-      </c>
-      <c r="I4" s="101">
-        <v>0</v>
-      </c>
-      <c r="J4" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="101" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="101">
-        <v>0</v>
-      </c>
-      <c r="D5" s="101">
-        <v>0</v>
-      </c>
-      <c r="E5" s="101">
-        <v>0.123</v>
-      </c>
-      <c r="F5" s="101">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="G5" s="101">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="H5" s="101">
+      <c r="I17" s="98">
+        <v>0</v>
+      </c>
+      <c r="J17" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="98" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="98">
+        <v>0</v>
+      </c>
+      <c r="D18" s="98">
+        <v>0</v>
+      </c>
+      <c r="E18" s="98">
+        <v>0.33</v>
+      </c>
+      <c r="F18" s="98">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G18" s="98">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="H18" s="98">
         <v>32</v>
       </c>
-      <c r="I5" s="101">
-        <v>0</v>
-      </c>
-      <c r="J5" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="101" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="101">
-        <v>0</v>
-      </c>
-      <c r="D6" s="101">
-        <v>0</v>
-      </c>
-      <c r="E6" s="101">
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="F6" s="101">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="G6" s="101">
-        <v>0.128</v>
-      </c>
-      <c r="H6" s="101">
-        <v>98</v>
-      </c>
-      <c r="I6" s="101">
-        <v>0</v>
-      </c>
-      <c r="J6" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="101" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" s="101">
-        <v>0</v>
-      </c>
-      <c r="D7" s="101">
-        <v>0</v>
-      </c>
-      <c r="E7" s="101">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="F7" s="101">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G7" s="101">
-        <v>0.107</v>
-      </c>
-      <c r="H7" s="101">
-        <v>136</v>
-      </c>
-      <c r="I7" s="101">
-        <v>0</v>
-      </c>
-      <c r="J7" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="101" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="101">
-        <v>0</v>
-      </c>
-      <c r="D8" s="101">
-        <v>0</v>
-      </c>
-      <c r="E8" s="101">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="F8" s="101">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="G8" s="101">
-        <v>0.1</v>
-      </c>
-      <c r="H8" s="101">
-        <v>107</v>
-      </c>
-      <c r="I8" s="101">
-        <v>0</v>
-      </c>
-      <c r="J8" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="101" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="101">
-        <v>0</v>
-      </c>
-      <c r="D9" s="101">
-        <v>0</v>
-      </c>
-      <c r="E9" s="101">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F9" s="101">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="G9" s="101">
-        <v>6.3E-2</v>
-      </c>
-      <c r="H9" s="101">
-        <v>32</v>
-      </c>
-      <c r="I9" s="101">
-        <v>0</v>
-      </c>
-      <c r="J9" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="101" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="101">
-        <v>0</v>
-      </c>
-      <c r="D10" s="101">
-        <v>0</v>
-      </c>
-      <c r="E10" s="101">
-        <v>0.105</v>
-      </c>
-      <c r="F10" s="101">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="G10" s="101">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="H10" s="101">
-        <v>169</v>
-      </c>
-      <c r="I10" s="101">
-        <v>0</v>
-      </c>
-      <c r="J10" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="101" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="101">
-        <v>0</v>
-      </c>
-      <c r="D11" s="101">
-        <v>0</v>
-      </c>
-      <c r="E11" s="101">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="F11" s="101">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="G11" s="101">
-        <v>6.2E-2</v>
-      </c>
-      <c r="H11" s="101">
-        <v>58</v>
-      </c>
-      <c r="I11" s="101">
-        <v>0</v>
-      </c>
-      <c r="J11" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="101" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="101">
-        <v>0</v>
-      </c>
-      <c r="D12" s="101">
-        <v>0</v>
-      </c>
-      <c r="E12" s="101">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="F12" s="101">
-        <v>0.01</v>
-      </c>
-      <c r="G12" s="101">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="H12" s="101">
-        <v>32</v>
-      </c>
-      <c r="I12" s="101">
-        <v>0</v>
-      </c>
-      <c r="J12" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="101" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="101">
-        <v>0</v>
-      </c>
-      <c r="D13" s="101">
-        <v>0</v>
-      </c>
-      <c r="E13" s="101">
-        <v>0.154</v>
-      </c>
-      <c r="F13" s="101">
-        <v>1.6E-2</v>
-      </c>
-      <c r="G13" s="101">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="H13" s="101">
-        <v>98</v>
-      </c>
-      <c r="I13" s="101">
-        <v>0</v>
-      </c>
-      <c r="J13" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="101" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="101">
-        <v>0</v>
-      </c>
-      <c r="D14" s="101">
-        <v>0</v>
-      </c>
-      <c r="E14" s="101">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="F14" s="101">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="G14" s="101">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="H14" s="101">
-        <v>14</v>
-      </c>
-      <c r="I14" s="101">
-        <v>0</v>
-      </c>
-      <c r="J14" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="101" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="101">
-        <v>0</v>
-      </c>
-      <c r="D15" s="101">
-        <v>0</v>
-      </c>
-      <c r="E15" s="101">
-        <v>0.33700000000000002</v>
-      </c>
-      <c r="F15" s="101">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="G15" s="101">
-        <v>0.33700000000000002</v>
-      </c>
-      <c r="H15" s="101">
-        <v>6</v>
-      </c>
-      <c r="I15" s="101">
-        <v>0</v>
-      </c>
-      <c r="J15" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="101" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="101">
-        <v>0</v>
-      </c>
-      <c r="D16" s="101">
-        <v>0</v>
-      </c>
-      <c r="E16" s="101">
-        <v>0.72799999999999998</v>
-      </c>
-      <c r="F16" s="101">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="G16" s="101">
-        <v>0.68400000000000005</v>
-      </c>
-      <c r="H16" s="101">
-        <v>59</v>
-      </c>
-      <c r="I16" s="101">
-        <v>0</v>
-      </c>
-      <c r="J16" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="101" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="101">
-        <v>0</v>
-      </c>
-      <c r="D17" s="101">
-        <v>0</v>
-      </c>
-      <c r="E17" s="101">
-        <v>0.36899999999999999</v>
-      </c>
-      <c r="F17" s="101">
-        <v>3.1E-2</v>
-      </c>
-      <c r="G17" s="101">
-        <v>0.36</v>
-      </c>
-      <c r="H17" s="101">
-        <v>24</v>
-      </c>
-      <c r="I17" s="101">
-        <v>0</v>
-      </c>
-      <c r="J17" s="101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="101" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="101">
-        <v>0</v>
-      </c>
-      <c r="D18" s="101">
-        <v>0</v>
-      </c>
-      <c r="E18" s="101">
-        <v>0.33</v>
-      </c>
-      <c r="F18" s="101">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="G18" s="101">
-        <v>0.29299999999999998</v>
-      </c>
-      <c r="H18" s="101">
-        <v>32</v>
-      </c>
-      <c r="I18" s="101">
-        <v>0</v>
-      </c>
-      <c r="J18" s="101">
+      <c r="I18" s="98">
+        <v>0</v>
+      </c>
+      <c r="J18" s="98">
         <v>0</v>
       </c>
       <c r="N18" s="91"/>
@@ -5527,34 +5556,34 @@
       <c r="V18" s="91"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="101" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="101">
-        <v>0</v>
-      </c>
-      <c r="D19" s="101">
-        <v>0</v>
-      </c>
-      <c r="E19" s="101">
+      <c r="A19" s="98" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="98">
+        <v>0</v>
+      </c>
+      <c r="D19" s="98">
+        <v>0</v>
+      </c>
+      <c r="E19" s="98">
         <v>0.59799999999999998</v>
       </c>
-      <c r="F19" s="101">
+      <c r="F19" s="98">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G19" s="101">
+      <c r="G19" s="98">
         <v>0.53200000000000003</v>
       </c>
-      <c r="H19" s="101">
+      <c r="H19" s="98">
         <v>34</v>
       </c>
-      <c r="I19" s="101">
-        <v>0</v>
-      </c>
-      <c r="J19" s="101">
+      <c r="I19" s="98">
+        <v>0</v>
+      </c>
+      <c r="J19" s="98">
         <v>0</v>
       </c>
       <c r="N19" s="91"/>
@@ -5837,13 +5866,13 @@
   </cols>
   <sheetData>
     <row r="9" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="100" t="s">
+      <c r="E9" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="100"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="100"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
     </row>
     <row r="11" spans="5:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
@@ -5996,13 +6025,13 @@
       </c>
     </row>
     <row r="23" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E23" s="100" t="s">
+      <c r="E23" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="100"/>
-      <c r="G23" s="100"/>
-      <c r="H23" s="100"/>
-      <c r="I23" s="100"/>
+      <c r="F23" s="101"/>
+      <c r="G23" s="101"/>
+      <c r="H23" s="101"/>
+      <c r="I23" s="101"/>
     </row>
     <row r="25" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E25" s="8" t="s">
@@ -6162,13 +6191,13 @@
       </c>
     </row>
     <row r="35" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E35" s="100" t="s">
+      <c r="E35" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="100"/>
-      <c r="G35" s="100"/>
-      <c r="H35" s="100"/>
-      <c r="I35" s="100"/>
+      <c r="F35" s="101"/>
+      <c r="G35" s="101"/>
+      <c r="H35" s="101"/>
+      <c r="I35" s="101"/>
     </row>
     <row r="37" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E37" s="8" t="s">

</xml_diff>